<commit_message>
a couple of genera added
</commit_message>
<xml_diff>
--- a/output/nla_phyto_taxonomy.xlsx
+++ b/output/nla_phyto_taxonomy.xlsx
@@ -19,7 +19,7 @@
     <sheet name="confusions" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nla_phyto_taxonomy!$A$1:$O$360</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nla_phyto_taxonomy!$A$1:$O$364</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">toxins!$A$1:$J$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">toxLoftin!$A$1:$F$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">toxPaerl!$A$1:$G$13</definedName>
@@ -293,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3543" uniqueCount="1366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3574" uniqueCount="1372">
   <si>
     <t>phylum</t>
   </si>
@@ -4121,9 +4121,6 @@
   </si>
   <si>
     <t>genus shown as "Sphaerodinium/Glenodinium/Peridiniopsis Complex" in 2007; changed to "Sphaerodinium"</t>
-  </si>
-  <si>
-    <t>Staurodesmus/Arthrodesmus/Octacanthium,"Staurodesmus"</t>
   </si>
   <si>
     <t>Teiling, 1948</t>
@@ -4694,6 +4691,27 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>Staurodesmus/Arthrodesmus/Octacanthium</t>
+  </si>
+  <si>
+    <t>Jaaginema</t>
+  </si>
+  <si>
+    <t>Karayevia</t>
+  </si>
+  <si>
+    <t>http://algaebase.org/search/genus/detail/?genus_id=Q607d9e6637155eee&amp;-session=abv4:CC2E5C920ecc92CA46KJD7A08040</t>
+  </si>
+  <si>
+    <t>Round &amp; L.Bukhtiyarova ex Round, 1998</t>
+  </si>
+  <si>
+    <t>http://algaebase.org/search/genus/detail/?genus_id=Ra066cdda960b1452&amp;-session=abv4:CC2E5C920ecc92CA46KJD7A08040</t>
+  </si>
+  <si>
+    <t>Jaaginema; Jaaginema metaphyticum</t>
   </si>
 </sst>
 </file>
@@ -5745,11 +5763,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O360"/>
+  <dimension ref="A1:O364"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A186" sqref="A186:XFD188"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K365" sqref="K365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5808,10 +5826,10 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="O1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -6422,7 +6440,7 @@
         <v>29</v>
       </c>
       <c r="N20" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O20" t="s">
         <v>30</v>
@@ -8559,10 +8577,10 @@
         <v>34</v>
       </c>
       <c r="M91" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="O91" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
@@ -15181,13 +15199,13 @@
         <v>815</v>
       </c>
       <c r="G315" t="s">
-        <v>1276</v>
+        <v>1018</v>
       </c>
       <c r="H315" t="s">
         <v>1018</v>
       </c>
       <c r="I315" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="J315" s="1" t="s">
         <v>34</v>
@@ -15198,34 +15216,31 @@
     </row>
     <row r="316" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>253</v>
-      </c>
-      <c r="B316" t="s">
-        <v>262</v>
+        <v>812</v>
       </c>
       <c r="C316" t="s">
-        <v>300</v>
-      </c>
-      <c r="D316" t="s">
-        <v>301</v>
+        <v>813</v>
       </c>
       <c r="E316" t="s">
-        <v>327</v>
+        <v>814</v>
       </c>
       <c r="F316" t="s">
-        <v>488</v>
+        <v>815</v>
       </c>
       <c r="G316" t="s">
-        <v>492</v>
+        <v>1365</v>
+      </c>
+      <c r="H316" t="s">
+        <v>1018</v>
       </c>
       <c r="I316" t="s">
-        <v>284</v>
+        <v>1276</v>
       </c>
       <c r="J316" s="1" t="s">
-        <v>492</v>
+        <v>34</v>
       </c>
       <c r="K316" s="1" t="s">
-        <v>493</v>
+        <v>34</v>
       </c>
     </row>
     <row r="317" spans="1:15" x14ac:dyDescent="0.25">
@@ -15239,25 +15254,25 @@
         <v>300</v>
       </c>
       <c r="D317" t="s">
-        <v>374</v>
+        <v>301</v>
       </c>
       <c r="E317" t="s">
-        <v>393</v>
+        <v>327</v>
       </c>
       <c r="F317" t="s">
-        <v>394</v>
+        <v>488</v>
       </c>
       <c r="G317" t="s">
-        <v>407</v>
+        <v>492</v>
       </c>
       <c r="I317" t="s">
         <v>284</v>
       </c>
       <c r="J317" s="1" t="s">
-        <v>408</v>
+        <v>492</v>
       </c>
       <c r="K317" s="1" t="s">
-        <v>408</v>
+        <v>493</v>
       </c>
     </row>
     <row r="318" spans="1:15" x14ac:dyDescent="0.25">
@@ -15280,16 +15295,16 @@
         <v>394</v>
       </c>
       <c r="G318" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I318" t="s">
-        <v>410</v>
+        <v>284</v>
       </c>
       <c r="J318" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K318" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="319" spans="1:15" x14ac:dyDescent="0.25">
@@ -15303,31 +15318,28 @@
         <v>300</v>
       </c>
       <c r="D319" t="s">
-        <v>301</v>
+        <v>374</v>
       </c>
       <c r="E319" t="s">
-        <v>443</v>
+        <v>393</v>
       </c>
       <c r="F319" t="s">
-        <v>494</v>
+        <v>394</v>
       </c>
       <c r="G319" t="s">
-        <v>500</v>
+        <v>409</v>
       </c>
       <c r="I319" t="s">
-        <v>501</v>
+        <v>410</v>
       </c>
       <c r="J319" s="1" t="s">
-        <v>502</v>
+        <v>409</v>
       </c>
       <c r="K319" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="O319" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="320" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="320" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>253</v>
       </c>
@@ -15335,260 +15347,266 @@
         <v>262</v>
       </c>
       <c r="C320" t="s">
+        <v>300</v>
+      </c>
+      <c r="D320" t="s">
+        <v>301</v>
+      </c>
+      <c r="E320" t="s">
+        <v>443</v>
+      </c>
+      <c r="F320" t="s">
+        <v>494</v>
+      </c>
+      <c r="G320" t="s">
+        <v>500</v>
+      </c>
+      <c r="I320" t="s">
+        <v>501</v>
+      </c>
+      <c r="J320" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="K320" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="O320" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="321" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>253</v>
+      </c>
+      <c r="B321" t="s">
+        <v>262</v>
+      </c>
+      <c r="C321" t="s">
         <v>263</v>
       </c>
-      <c r="D320" t="s">
+      <c r="D321" t="s">
         <v>286</v>
       </c>
-      <c r="E320" t="s">
+      <c r="E321" t="s">
         <v>287</v>
       </c>
-      <c r="F320" t="s">
+      <c r="F321" t="s">
         <v>288</v>
       </c>
-      <c r="G320" t="s">
+      <c r="G321" t="s">
         <v>297</v>
       </c>
-      <c r="I320" t="s">
+      <c r="I321" t="s">
         <v>298</v>
       </c>
-      <c r="J320" s="1" t="s">
+      <c r="J321" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="K320" s="1" t="s">
+      <c r="K321" s="1" t="s">
         <v>299</v>
-      </c>
-    </row>
-    <row r="321" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A321" t="s">
-        <v>596</v>
-      </c>
-      <c r="C321" t="s">
-        <v>927</v>
-      </c>
-      <c r="E321" t="s">
-        <v>928</v>
-      </c>
-      <c r="F321" t="s">
-        <v>929</v>
-      </c>
-      <c r="G321" t="s">
-        <v>930</v>
-      </c>
-      <c r="I321" t="s">
-        <v>931</v>
-      </c>
-      <c r="J321" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K321" s="1" t="s">
-        <v>930</v>
       </c>
     </row>
     <row r="322" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>13</v>
+        <v>596</v>
       </c>
       <c r="C322" t="s">
-        <v>14</v>
-      </c>
-      <c r="D322" t="s">
-        <v>23</v>
+        <v>927</v>
       </c>
       <c r="E322" t="s">
-        <v>24</v>
+        <v>928</v>
       </c>
       <c r="F322" t="s">
-        <v>1077</v>
+        <v>929</v>
       </c>
       <c r="G322" t="s">
-        <v>1078</v>
+        <v>930</v>
       </c>
       <c r="I322" t="s">
-        <v>1079</v>
+        <v>931</v>
       </c>
       <c r="J322" s="1" t="s">
-        <v>1078</v>
+        <v>34</v>
       </c>
       <c r="K322" s="1" t="s">
-        <v>34</v>
+        <v>930</v>
       </c>
     </row>
     <row r="323" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>659</v>
-      </c>
-      <c r="B323" t="s">
-        <v>660</v>
+        <v>13</v>
       </c>
       <c r="C323" t="s">
-        <v>682</v>
+        <v>14</v>
+      </c>
+      <c r="D323" t="s">
+        <v>23</v>
       </c>
       <c r="E323" t="s">
-        <v>1170</v>
+        <v>24</v>
       </c>
       <c r="F323" t="s">
-        <v>1171</v>
+        <v>1077</v>
       </c>
       <c r="G323" t="s">
-        <v>1173</v>
+        <v>1078</v>
       </c>
       <c r="I323" t="s">
-        <v>1174</v>
+        <v>1079</v>
       </c>
       <c r="J323" s="1" t="s">
-        <v>1173</v>
+        <v>1078</v>
       </c>
       <c r="K323" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="O323" t="s">
-        <v>1175</v>
       </c>
     </row>
     <row r="324" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
+        <v>659</v>
+      </c>
+      <c r="B324" t="s">
+        <v>660</v>
+      </c>
+      <c r="C324" t="s">
+        <v>682</v>
+      </c>
+      <c r="E324" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F324" t="s">
+        <v>1171</v>
+      </c>
+      <c r="G324" t="s">
+        <v>1173</v>
+      </c>
+      <c r="I324" t="s">
+        <v>1174</v>
+      </c>
+      <c r="J324" s="1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="K324" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O324" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="325" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
         <v>596</v>
       </c>
-      <c r="C324" t="s">
+      <c r="C325" t="s">
         <v>927</v>
       </c>
-      <c r="E324" t="s">
+      <c r="E325" t="s">
         <v>928</v>
       </c>
-      <c r="F324" t="s">
+      <c r="F325" t="s">
         <v>929</v>
       </c>
-      <c r="G324" t="s">
+      <c r="G325" t="s">
         <v>1272</v>
       </c>
-      <c r="I324" t="s">
+      <c r="I325" t="s">
         <v>931</v>
       </c>
-      <c r="J324" s="1" t="s">
+      <c r="J325" s="1" t="s">
         <v>1272</v>
       </c>
-      <c r="K324" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="325" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A325" t="s">
+      <c r="K325" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="326" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
         <v>567</v>
       </c>
-      <c r="B325" t="s">
+      <c r="B326" t="s">
         <v>568</v>
       </c>
-      <c r="C325" t="s">
+      <c r="C326" t="s">
         <v>569</v>
       </c>
-      <c r="E325" t="s">
+      <c r="E326" t="s">
         <v>570</v>
       </c>
-      <c r="F325" t="s">
+      <c r="F326" t="s">
         <v>571</v>
       </c>
-      <c r="G325" t="s">
+      <c r="G326" t="s">
         <v>586</v>
       </c>
-      <c r="I325" t="s">
+      <c r="I326" t="s">
         <v>587</v>
       </c>
-      <c r="J325" s="1" t="s">
+      <c r="J326" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="K325" s="1" t="s">
+      <c r="K326" s="1" t="s">
         <v>588</v>
-      </c>
-    </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A326" t="s">
-        <v>596</v>
-      </c>
-      <c r="C326" t="s">
-        <v>604</v>
-      </c>
-      <c r="E326" t="s">
-        <v>605</v>
-      </c>
-      <c r="F326" t="s">
-        <v>610</v>
-      </c>
-      <c r="G326" t="s">
-        <v>1248</v>
-      </c>
-      <c r="I326" t="s">
-        <v>955</v>
-      </c>
-      <c r="J326" s="1" t="s">
-        <v>1248</v>
-      </c>
-      <c r="K326" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="327" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
+        <v>596</v>
+      </c>
+      <c r="C327" t="s">
+        <v>604</v>
+      </c>
+      <c r="E327" t="s">
+        <v>605</v>
+      </c>
+      <c r="F327" t="s">
+        <v>610</v>
+      </c>
+      <c r="G327" t="s">
+        <v>1248</v>
+      </c>
+      <c r="I327" t="s">
+        <v>955</v>
+      </c>
+      <c r="J327" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="K327" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="328" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
         <v>253</v>
       </c>
-      <c r="B327" t="s">
+      <c r="B328" t="s">
         <v>262</v>
       </c>
-      <c r="C327" t="s">
+      <c r="C328" t="s">
         <v>300</v>
       </c>
-      <c r="D327" t="s">
+      <c r="D328" t="s">
         <v>301</v>
       </c>
-      <c r="E327" t="s">
+      <c r="E328" t="s">
         <v>443</v>
       </c>
-      <c r="F327" t="s">
+      <c r="F328" t="s">
         <v>494</v>
       </c>
-      <c r="G327" t="s">
+      <c r="G328" t="s">
         <v>504</v>
       </c>
-      <c r="I327" t="s">
+      <c r="I328" t="s">
         <v>505</v>
       </c>
-      <c r="J327" s="1" t="s">
+      <c r="J328" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="K327" s="1" t="s">
+      <c r="K328" s="1" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="328" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A328" t="s">
-        <v>13</v>
-      </c>
-      <c r="C328" t="s">
-        <v>14</v>
-      </c>
-      <c r="D328" t="s">
-        <v>15</v>
-      </c>
-      <c r="E328" t="s">
-        <v>16</v>
-      </c>
-      <c r="F328" t="s">
-        <v>105</v>
-      </c>
-      <c r="G328" t="s">
-        <v>106</v>
-      </c>
-      <c r="I328" t="s">
-        <v>19</v>
-      </c>
-      <c r="J328" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K328" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="329" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>13</v>
       </c>
@@ -15602,115 +15620,109 @@
         <v>16</v>
       </c>
       <c r="F329" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="G329" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="I329" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="J329" s="1" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="K329" s="1" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
     </row>
     <row r="330" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
+        <v>13</v>
+      </c>
+      <c r="C330" t="s">
+        <v>14</v>
+      </c>
+      <c r="D330" t="s">
+        <v>15</v>
+      </c>
+      <c r="E330" t="s">
+        <v>16</v>
+      </c>
+      <c r="F330" t="s">
+        <v>17</v>
+      </c>
+      <c r="G330" t="s">
+        <v>79</v>
+      </c>
+      <c r="I330" t="s">
+        <v>80</v>
+      </c>
+      <c r="J330" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K330" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="331" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
         <v>253</v>
       </c>
-      <c r="B330" t="s">
+      <c r="B331" t="s">
         <v>262</v>
       </c>
-      <c r="C330" t="s">
+      <c r="C331" t="s">
         <v>300</v>
       </c>
-      <c r="D330" t="s">
+      <c r="D331" t="s">
         <v>374</v>
       </c>
-      <c r="E330" t="s">
+      <c r="E331" t="s">
         <v>393</v>
       </c>
-      <c r="F330" t="s">
+      <c r="F331" t="s">
         <v>394</v>
       </c>
-      <c r="G330" t="s">
+      <c r="G331" t="s">
         <v>411</v>
       </c>
-      <c r="I330" t="s">
+      <c r="I331" t="s">
         <v>412</v>
       </c>
-      <c r="J330" s="1" t="s">
+      <c r="J331" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="K330" s="1" t="s">
+      <c r="K331" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="331" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A331" t="s">
+    <row r="332" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
         <v>596</v>
       </c>
-      <c r="C331" t="s">
+      <c r="C332" t="s">
         <v>627</v>
       </c>
-      <c r="E331" t="s">
+      <c r="E332" t="s">
         <v>628</v>
       </c>
-      <c r="F331" t="s">
+      <c r="F332" t="s">
         <v>632</v>
       </c>
-      <c r="G331" t="s">
+      <c r="G332" t="s">
         <v>633</v>
       </c>
-      <c r="I331" t="s">
+      <c r="I332" t="s">
         <v>624</v>
       </c>
-      <c r="J331" s="1" t="s">
+      <c r="J332" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="K331" s="1" t="s">
+      <c r="K332" s="1" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="332" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A332" t="s">
-        <v>253</v>
-      </c>
-      <c r="B332" t="s">
-        <v>262</v>
-      </c>
-      <c r="C332" t="s">
-        <v>300</v>
-      </c>
-      <c r="D332" t="s">
-        <v>374</v>
-      </c>
-      <c r="E332" t="s">
-        <v>380</v>
-      </c>
-      <c r="F332" t="s">
-        <v>381</v>
-      </c>
-      <c r="G332" t="s">
-        <v>507</v>
-      </c>
-      <c r="I332" t="s">
-        <v>365</v>
-      </c>
-      <c r="J332" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="K332" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="O332" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="333" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>253</v>
       </c>
@@ -15724,54 +15736,63 @@
         <v>374</v>
       </c>
       <c r="E333" t="s">
+        <v>380</v>
+      </c>
+      <c r="F333" t="s">
+        <v>381</v>
+      </c>
+      <c r="G333" t="s">
+        <v>507</v>
+      </c>
+      <c r="I333" t="s">
+        <v>365</v>
+      </c>
+      <c r="J333" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="K333" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="O333" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="334" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>253</v>
+      </c>
+      <c r="B334" t="s">
+        <v>262</v>
+      </c>
+      <c r="C334" t="s">
+        <v>300</v>
+      </c>
+      <c r="D334" t="s">
+        <v>374</v>
+      </c>
+      <c r="E334" t="s">
         <v>375</v>
       </c>
-      <c r="F333" t="s">
+      <c r="F334" t="s">
         <v>376</v>
       </c>
-      <c r="G333" t="s">
+      <c r="G334" t="s">
         <v>1150</v>
       </c>
-      <c r="I333" t="s">
+      <c r="I334" t="s">
         <v>1151</v>
       </c>
-      <c r="J333" s="1" t="s">
+      <c r="J334" s="1" t="s">
         <v>1150</v>
       </c>
-      <c r="K333" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O333" t="s">
+      <c r="K334" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O334" t="s">
         <v>1152</v>
       </c>
     </row>
-    <row r="334" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A334" t="s">
-        <v>812</v>
-      </c>
-      <c r="C334" t="s">
-        <v>813</v>
-      </c>
-      <c r="E334" t="s">
-        <v>814</v>
-      </c>
-      <c r="F334" t="s">
-        <v>815</v>
-      </c>
-      <c r="G334" t="s">
-        <v>1019</v>
-      </c>
-      <c r="I334" t="s">
-        <v>1020</v>
-      </c>
-      <c r="J334" s="1" t="s">
-        <v>1019</v>
-      </c>
-      <c r="K334" s="1" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="335" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>812</v>
       </c>
@@ -15785,112 +15806,103 @@
         <v>815</v>
       </c>
       <c r="G335" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="I335" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="J335" s="1" t="s">
-        <v>34</v>
+        <v>1019</v>
       </c>
       <c r="K335" s="1" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="336" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
+        <v>812</v>
+      </c>
+      <c r="C336" t="s">
+        <v>813</v>
+      </c>
+      <c r="E336" t="s">
+        <v>814</v>
+      </c>
+      <c r="F336" t="s">
+        <v>815</v>
+      </c>
+      <c r="G336" t="s">
+        <v>1022</v>
+      </c>
+      <c r="I336" t="s">
+        <v>1023</v>
+      </c>
+      <c r="J336" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K336" s="1" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="337" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
         <v>659</v>
       </c>
-      <c r="B336" t="s">
+      <c r="B337" t="s">
         <v>660</v>
       </c>
-      <c r="C336" t="s">
+      <c r="C337" t="s">
         <v>682</v>
       </c>
-      <c r="E336" t="s">
+      <c r="E337" t="s">
         <v>683</v>
       </c>
-      <c r="F336" t="s">
+      <c r="F337" t="s">
         <v>778</v>
       </c>
-      <c r="G336" t="s">
+      <c r="G337" t="s">
         <v>860</v>
       </c>
-      <c r="I336" t="s">
+      <c r="I337" t="s">
         <v>861</v>
       </c>
-      <c r="J336" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K336" s="1" t="s">
+      <c r="J337" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K337" s="1" t="s">
         <v>862</v>
       </c>
-      <c r="O336" t="s">
+      <c r="O337" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="337" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A337" t="s">
+    <row r="338" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
         <v>596</v>
       </c>
-      <c r="C337" t="s">
+      <c r="C338" t="s">
         <v>597</v>
       </c>
-      <c r="E337" t="s">
+      <c r="E338" t="s">
         <v>598</v>
       </c>
-      <c r="F337" t="s">
+      <c r="F338" t="s">
         <v>599</v>
       </c>
-      <c r="G337" t="s">
+      <c r="G338" t="s">
         <v>1073</v>
       </c>
-      <c r="I337" t="s">
+      <c r="I338" t="s">
         <v>1071</v>
       </c>
-      <c r="J337" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K337" s="1" t="s">
+      <c r="J338" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K338" s="1" t="s">
         <v>1074</v>
       </c>
     </row>
-    <row r="338" spans="1:15" ht="195" x14ac:dyDescent="0.25">
-      <c r="A338" t="s">
-        <v>659</v>
-      </c>
-      <c r="B338" t="s">
-        <v>660</v>
-      </c>
-      <c r="C338" t="s">
-        <v>682</v>
-      </c>
-      <c r="E338" t="s">
-        <v>683</v>
-      </c>
-      <c r="F338" t="s">
-        <v>695</v>
-      </c>
-      <c r="G338" t="s">
-        <v>696</v>
-      </c>
-      <c r="H338" t="s">
-        <v>697</v>
-      </c>
-      <c r="I338" t="s">
-        <v>698</v>
-      </c>
-      <c r="J338" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K338" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="M338" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="339" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:15" ht="195" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>659</v>
       </c>
@@ -15907,22 +15919,25 @@
         <v>695</v>
       </c>
       <c r="G339" t="s">
+        <v>696</v>
+      </c>
+      <c r="H339" t="s">
         <v>697</v>
       </c>
       <c r="I339" t="s">
         <v>698</v>
       </c>
       <c r="J339" s="1" t="s">
-        <v>1176</v>
+        <v>34</v>
       </c>
       <c r="K339" s="1" t="s">
-        <v>34</v>
+        <v>699</v>
       </c>
       <c r="M339" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="340" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>659</v>
       </c>
@@ -15936,19 +15951,22 @@
         <v>683</v>
       </c>
       <c r="F340" t="s">
-        <v>778</v>
+        <v>695</v>
       </c>
       <c r="G340" t="s">
-        <v>864</v>
+        <v>697</v>
       </c>
       <c r="I340" t="s">
-        <v>865</v>
+        <v>698</v>
       </c>
       <c r="J340" s="1" t="s">
-        <v>34</v>
+        <v>1176</v>
       </c>
       <c r="K340" s="1" t="s">
-        <v>866</v>
+        <v>34</v>
+      </c>
+      <c r="M340" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="341" spans="1:15" x14ac:dyDescent="0.25">
@@ -15959,28 +15977,28 @@
         <v>660</v>
       </c>
       <c r="C341" t="s">
-        <v>962</v>
+        <v>682</v>
       </c>
       <c r="E341" t="s">
-        <v>963</v>
+        <v>683</v>
       </c>
       <c r="F341" t="s">
-        <v>964</v>
+        <v>778</v>
       </c>
       <c r="G341" t="s">
-        <v>965</v>
+        <v>864</v>
       </c>
       <c r="I341" t="s">
-        <v>534</v>
+        <v>865</v>
       </c>
       <c r="J341" s="1" t="s">
-        <v>965</v>
+        <v>34</v>
       </c>
       <c r="K341" s="1" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="342" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="342" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>659</v>
       </c>
@@ -15988,434 +16006,434 @@
         <v>660</v>
       </c>
       <c r="C342" t="s">
+        <v>962</v>
+      </c>
+      <c r="E342" t="s">
+        <v>963</v>
+      </c>
+      <c r="F342" t="s">
+        <v>964</v>
+      </c>
+      <c r="G342" t="s">
+        <v>965</v>
+      </c>
+      <c r="I342" t="s">
+        <v>534</v>
+      </c>
+      <c r="J342" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="K342" s="1" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="343" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>659</v>
+      </c>
+      <c r="B343" t="s">
+        <v>660</v>
+      </c>
+      <c r="C343" t="s">
         <v>682</v>
       </c>
-      <c r="E342" t="s">
+      <c r="E343" t="s">
         <v>683</v>
       </c>
-      <c r="F342" t="s">
+      <c r="F343" t="s">
         <v>778</v>
       </c>
-      <c r="G342" t="s">
+      <c r="G343" t="s">
         <v>799</v>
       </c>
-      <c r="I342" t="s">
+      <c r="I343" t="s">
         <v>749</v>
       </c>
-      <c r="J342" s="1" t="s">
+      <c r="J343" s="1" t="s">
         <v>800</v>
       </c>
-      <c r="K342" s="1" t="s">
+      <c r="K343" s="1" t="s">
         <v>801</v>
-      </c>
-    </row>
-    <row r="343" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A343" t="s">
-        <v>253</v>
-      </c>
-      <c r="B343" t="s">
-        <v>262</v>
-      </c>
-      <c r="C343" t="s">
-        <v>263</v>
-      </c>
-      <c r="D343" t="s">
-        <v>286</v>
-      </c>
-      <c r="E343" t="s">
-        <v>1127</v>
-      </c>
-      <c r="F343" t="s">
-        <v>1136</v>
-      </c>
-      <c r="G343" t="s">
-        <v>1137</v>
-      </c>
-      <c r="I343" t="s">
-        <v>1138</v>
-      </c>
-      <c r="J343" s="1" t="s">
-        <v>1137</v>
-      </c>
-      <c r="K343" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="344" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
+        <v>253</v>
+      </c>
+      <c r="B344" t="s">
+        <v>262</v>
+      </c>
+      <c r="C344" t="s">
+        <v>263</v>
+      </c>
+      <c r="D344" t="s">
+        <v>286</v>
+      </c>
+      <c r="E344" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F344" t="s">
+        <v>1136</v>
+      </c>
+      <c r="G344" t="s">
+        <v>1137</v>
+      </c>
+      <c r="I344" t="s">
+        <v>1138</v>
+      </c>
+      <c r="J344" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="K344" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="345" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
         <v>13</v>
       </c>
-      <c r="C344" t="s">
+      <c r="C345" t="s">
         <v>14</v>
       </c>
-      <c r="D344" t="s">
+      <c r="D345" t="s">
         <v>109</v>
       </c>
-      <c r="E344" t="s">
+      <c r="E345" t="s">
         <v>110</v>
       </c>
-      <c r="F344" t="s">
+      <c r="F345" t="s">
         <v>111</v>
       </c>
-      <c r="G344" t="s">
+      <c r="G345" t="s">
         <v>112</v>
       </c>
-      <c r="I344" t="s">
+      <c r="I345" t="s">
         <v>113</v>
       </c>
-      <c r="J344" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K344" s="1" t="s">
+      <c r="J345" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K345" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="345" spans="1:15" ht="225" x14ac:dyDescent="0.25">
-      <c r="A345" t="s">
+    <row r="346" spans="1:15" ht="225" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
         <v>567</v>
       </c>
-      <c r="B345" t="s">
+      <c r="B346" t="s">
         <v>568</v>
       </c>
-      <c r="C345" t="s">
+      <c r="C346" t="s">
         <v>569</v>
       </c>
-      <c r="E345" t="s">
+      <c r="E346" t="s">
         <v>570</v>
       </c>
-      <c r="F345" t="s">
+      <c r="F346" t="s">
         <v>571</v>
       </c>
-      <c r="G345" t="s">
+      <c r="G346" t="s">
         <v>589</v>
       </c>
-      <c r="I345" t="s">
+      <c r="I346" t="s">
         <v>590</v>
       </c>
-      <c r="J345" s="1" t="s">
+      <c r="J346" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="K345" s="1" t="s">
+      <c r="K346" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="O345" t="s">
+      <c r="O346" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="346" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A346" t="s">
+    <row r="347" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
         <v>659</v>
       </c>
-      <c r="B346" t="s">
+      <c r="B347" t="s">
         <v>660</v>
       </c>
-      <c r="C346" t="s">
+      <c r="C347" t="s">
         <v>682</v>
       </c>
-      <c r="E346" t="s">
+      <c r="E347" t="s">
         <v>689</v>
       </c>
-      <c r="F346" t="s">
+      <c r="F347" t="s">
         <v>836</v>
       </c>
-      <c r="G346" t="s">
+      <c r="G347" t="s">
         <v>837</v>
       </c>
-      <c r="I346" t="s">
+      <c r="I347" t="s">
         <v>838</v>
       </c>
-      <c r="J346" s="1" t="s">
+      <c r="J347" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="K346" s="1" t="s">
+      <c r="K347" s="1" t="s">
         <v>839</v>
-      </c>
-    </row>
-    <row r="347" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A347" t="s">
-        <v>596</v>
-      </c>
-      <c r="C347" t="s">
-        <v>927</v>
-      </c>
-      <c r="E347" t="s">
-        <v>1047</v>
-      </c>
-      <c r="F347" t="s">
-        <v>1048</v>
-      </c>
-      <c r="G347" t="s">
-        <v>1049</v>
-      </c>
-      <c r="I347" t="s">
-        <v>1050</v>
-      </c>
-      <c r="J347" s="1" t="s">
-        <v>1049</v>
-      </c>
-      <c r="K347" s="1" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="348" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>13</v>
+        <v>596</v>
       </c>
       <c r="C348" t="s">
-        <v>14</v>
-      </c>
-      <c r="D348" t="s">
-        <v>23</v>
+        <v>927</v>
       </c>
       <c r="E348" t="s">
-        <v>92</v>
+        <v>1047</v>
       </c>
       <c r="F348" t="s">
-        <v>145</v>
+        <v>1048</v>
       </c>
       <c r="G348" t="s">
-        <v>178</v>
+        <v>1049</v>
       </c>
       <c r="I348" t="s">
-        <v>179</v>
+        <v>1050</v>
       </c>
       <c r="J348" s="1" t="s">
-        <v>178</v>
+        <v>1049</v>
       </c>
       <c r="K348" s="1" t="s">
-        <v>180</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="349" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>659</v>
-      </c>
-      <c r="B349" t="s">
-        <v>660</v>
+        <v>13</v>
       </c>
       <c r="C349" t="s">
-        <v>661</v>
+        <v>14</v>
+      </c>
+      <c r="D349" t="s">
+        <v>23</v>
       </c>
       <c r="E349" t="s">
-        <v>662</v>
+        <v>92</v>
       </c>
       <c r="F349" t="s">
-        <v>738</v>
+        <v>145</v>
       </c>
       <c r="G349" t="s">
-        <v>1194</v>
+        <v>178</v>
       </c>
       <c r="I349" t="s">
-        <v>437</v>
+        <v>179</v>
       </c>
       <c r="J349" s="1" t="s">
-        <v>1194</v>
+        <v>178</v>
       </c>
       <c r="K349" s="1" t="s">
-        <v>34</v>
+        <v>180</v>
       </c>
     </row>
     <row r="350" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>253</v>
+        <v>659</v>
       </c>
       <c r="B350" t="s">
-        <v>262</v>
+        <v>660</v>
       </c>
       <c r="C350" t="s">
-        <v>300</v>
-      </c>
-      <c r="D350" t="s">
-        <v>301</v>
+        <v>661</v>
       </c>
       <c r="E350" t="s">
-        <v>341</v>
+        <v>662</v>
       </c>
       <c r="F350" t="s">
-        <v>342</v>
+        <v>738</v>
       </c>
       <c r="G350" t="s">
-        <v>357</v>
+        <v>1194</v>
       </c>
       <c r="I350" t="s">
-        <v>358</v>
+        <v>437</v>
       </c>
       <c r="J350" s="1" t="s">
-        <v>357</v>
+        <v>1194</v>
       </c>
       <c r="K350" s="1" t="s">
-        <v>357</v>
+        <v>34</v>
       </c>
     </row>
     <row r="351" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
+        <v>253</v>
+      </c>
+      <c r="B351" t="s">
+        <v>262</v>
+      </c>
+      <c r="C351" t="s">
+        <v>300</v>
+      </c>
+      <c r="D351" t="s">
+        <v>301</v>
+      </c>
+      <c r="E351" t="s">
+        <v>341</v>
+      </c>
+      <c r="F351" t="s">
+        <v>342</v>
+      </c>
+      <c r="G351" t="s">
+        <v>357</v>
+      </c>
+      <c r="I351" t="s">
+        <v>358</v>
+      </c>
+      <c r="J351" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="K351" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="352" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
         <v>13</v>
       </c>
-      <c r="C351" t="s">
+      <c r="C352" t="s">
         <v>14</v>
       </c>
-      <c r="D351" t="s">
+      <c r="D352" t="s">
         <v>23</v>
       </c>
-      <c r="E351" t="s">
+      <c r="E352" t="s">
         <v>92</v>
       </c>
-      <c r="F351" t="s">
+      <c r="F352" t="s">
         <v>145</v>
       </c>
-      <c r="G351" t="s">
+      <c r="G352" t="s">
         <v>181</v>
       </c>
-      <c r="I351" t="s">
+      <c r="I352" t="s">
         <v>161</v>
       </c>
-      <c r="J351" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K351" s="1" t="s">
+      <c r="J352" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K352" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="352" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
+    <row r="353" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
         <v>659</v>
       </c>
-      <c r="B352" t="s">
+      <c r="B353" t="s">
         <v>660</v>
       </c>
-      <c r="C352" t="s">
+      <c r="C353" t="s">
         <v>802</v>
       </c>
-      <c r="E352" t="s">
+      <c r="E353" t="s">
         <v>900</v>
       </c>
-      <c r="F352" t="s">
+      <c r="F353" t="s">
         <v>908</v>
       </c>
-      <c r="G352" t="s">
+      <c r="G353" t="s">
         <v>932</v>
       </c>
-      <c r="I352" t="s">
+      <c r="I353" t="s">
         <v>933</v>
       </c>
-      <c r="J352" s="1" t="s">
+      <c r="J353" s="1" t="s">
         <v>932</v>
       </c>
-      <c r="K352" s="1" t="s">
+      <c r="K353" s="1" t="s">
         <v>934</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A353" t="s">
+    <row r="354" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
         <v>596</v>
       </c>
-      <c r="C353" t="s">
+      <c r="C354" t="s">
         <v>604</v>
       </c>
-      <c r="E353" t="s">
+      <c r="E354" t="s">
         <v>605</v>
       </c>
-      <c r="F353" t="s">
+      <c r="F354" t="s">
         <v>606</v>
       </c>
-      <c r="G353" t="s">
+      <c r="G354" t="s">
         <v>642</v>
       </c>
-      <c r="I353" t="s">
+      <c r="I354" t="s">
         <v>624</v>
       </c>
-      <c r="J353" s="1" t="s">
+      <c r="J354" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="K353" s="1" t="s">
+      <c r="K354" s="1" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A354" t="s">
+    <row r="355" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
         <v>253</v>
       </c>
-      <c r="B354" t="s">
+      <c r="B355" t="s">
         <v>254</v>
       </c>
-      <c r="C354" t="s">
+      <c r="C355" t="s">
         <v>255</v>
       </c>
-      <c r="E354" t="s">
+      <c r="E355" t="s">
         <v>281</v>
       </c>
-      <c r="F354" t="s">
+      <c r="F355" t="s">
         <v>282</v>
       </c>
-      <c r="G354" t="s">
+      <c r="G355" t="s">
         <v>1125</v>
       </c>
-      <c r="I354" t="s">
+      <c r="I355" t="s">
         <v>1126</v>
       </c>
-      <c r="J354" s="1" t="s">
+      <c r="J355" s="1" t="s">
         <v>1125</v>
       </c>
-      <c r="K354" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A355" t="s">
+      <c r="K355" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="356" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
         <v>596</v>
       </c>
-      <c r="C355" t="s">
+      <c r="C356" t="s">
         <v>653</v>
       </c>
-      <c r="E355" t="s">
+      <c r="E356" t="s">
         <v>654</v>
       </c>
-      <c r="F355" t="s">
+      <c r="F356" t="s">
         <v>655</v>
       </c>
-      <c r="G355" t="s">
+      <c r="G356" t="s">
         <v>1239</v>
       </c>
-      <c r="I355" t="s">
+      <c r="I356" t="s">
         <v>1240</v>
       </c>
-      <c r="J355" s="1" t="s">
+      <c r="J356" s="1" t="s">
         <v>1239</v>
       </c>
-      <c r="K355" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A356" t="s">
-        <v>659</v>
-      </c>
-      <c r="B356" t="s">
-        <v>660</v>
-      </c>
-      <c r="C356" t="s">
-        <v>682</v>
-      </c>
-      <c r="E356" t="s">
-        <v>689</v>
-      </c>
-      <c r="F356" t="s">
-        <v>967</v>
-      </c>
-      <c r="G356" t="s">
-        <v>979</v>
-      </c>
-      <c r="I356" t="s">
-        <v>980</v>
-      </c>
-      <c r="J356" s="1" t="s">
-        <v>979</v>
-      </c>
       <c r="K356" s="1" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="357" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="357" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>659</v>
       </c>
@@ -16426,80 +16444,83 @@
         <v>682</v>
       </c>
       <c r="E357" t="s">
+        <v>689</v>
+      </c>
+      <c r="F357" t="s">
+        <v>967</v>
+      </c>
+      <c r="G357" t="s">
+        <v>979</v>
+      </c>
+      <c r="I357" t="s">
+        <v>980</v>
+      </c>
+      <c r="J357" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="K357" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="358" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>659</v>
+      </c>
+      <c r="B358" t="s">
+        <v>660</v>
+      </c>
+      <c r="C358" t="s">
+        <v>682</v>
+      </c>
+      <c r="E358" t="s">
         <v>683</v>
       </c>
-      <c r="F357" t="s">
+      <c r="F358" t="s">
         <v>778</v>
       </c>
-      <c r="G357" t="s">
+      <c r="G358" t="s">
         <v>779</v>
       </c>
-      <c r="I357" t="s">
+      <c r="I358" t="s">
         <v>780</v>
       </c>
-      <c r="J357" s="1" t="s">
+      <c r="J358" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="K357" s="1" t="s">
+      <c r="K358" s="1" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="358" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A358" t="s">
+    <row r="359" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
         <v>13</v>
       </c>
-      <c r="C358" t="s">
+      <c r="C359" t="s">
         <v>14</v>
       </c>
-      <c r="D358" t="s">
+      <c r="D359" t="s">
         <v>15</v>
       </c>
-      <c r="E358" t="s">
+      <c r="E359" t="s">
         <v>16</v>
       </c>
-      <c r="F358" t="s">
+      <c r="F359" t="s">
         <v>43</v>
       </c>
-      <c r="G358" t="s">
+      <c r="G359" t="s">
         <v>82</v>
       </c>
-      <c r="I358" t="s">
+      <c r="I359" t="s">
         <v>83</v>
       </c>
-      <c r="J358" s="1" t="s">
+      <c r="J359" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K358" s="1" t="s">
+      <c r="K359" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A359" t="s">
-        <v>812</v>
-      </c>
-      <c r="C359" t="s">
-        <v>813</v>
-      </c>
-      <c r="E359" t="s">
-        <v>814</v>
-      </c>
-      <c r="F359" t="s">
-        <v>815</v>
-      </c>
-      <c r="G359" t="s">
-        <v>1024</v>
-      </c>
-      <c r="I359" t="s">
-        <v>821</v>
-      </c>
-      <c r="J359" s="1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="K359" s="1" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>812</v>
       </c>
@@ -16507,28 +16528,130 @@
         <v>813</v>
       </c>
       <c r="E360" t="s">
+        <v>814</v>
+      </c>
+      <c r="F360" t="s">
+        <v>815</v>
+      </c>
+      <c r="G360" t="s">
+        <v>1024</v>
+      </c>
+      <c r="I360" t="s">
+        <v>821</v>
+      </c>
+      <c r="J360" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K360" s="1" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="361" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>812</v>
+      </c>
+      <c r="C361" t="s">
+        <v>813</v>
+      </c>
+      <c r="E361" t="s">
         <v>1029</v>
       </c>
-      <c r="F360" t="s">
+      <c r="F361" t="s">
         <v>1030</v>
       </c>
-      <c r="G360" t="s">
+      <c r="G361" t="s">
         <v>1035</v>
       </c>
-      <c r="I360" t="s">
+      <c r="I361" t="s">
         <v>826</v>
       </c>
-      <c r="J360" s="1" t="s">
+      <c r="J361" s="1" t="s">
         <v>1035</v>
       </c>
-      <c r="K360" s="1" t="s">
+      <c r="K361" s="1" t="s">
         <v>1035</v>
       </c>
     </row>
+    <row r="362" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G362" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="363" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>253</v>
+      </c>
+      <c r="B363" t="s">
+        <v>262</v>
+      </c>
+      <c r="C363" t="s">
+        <v>300</v>
+      </c>
+      <c r="D363" t="s">
+        <v>301</v>
+      </c>
+      <c r="E363" t="s">
+        <v>307</v>
+      </c>
+      <c r="F363" t="s">
+        <v>313</v>
+      </c>
+      <c r="G363" t="s">
+        <v>1367</v>
+      </c>
+      <c r="I363" t="s">
+        <v>1369</v>
+      </c>
+      <c r="J363" t="s">
+        <v>1367</v>
+      </c>
+      <c r="K363" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O363" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="364" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>13</v>
+      </c>
+      <c r="C364" t="s">
+        <v>14</v>
+      </c>
+      <c r="D364" t="s">
+        <v>15</v>
+      </c>
+      <c r="E364" t="s">
+        <v>16</v>
+      </c>
+      <c r="F364" t="s">
+        <v>193</v>
+      </c>
+      <c r="G364" t="s">
+        <v>1366</v>
+      </c>
+      <c r="I364" t="s">
+        <v>161</v>
+      </c>
+      <c r="J364" t="s">
+        <v>1366</v>
+      </c>
+      <c r="K364" t="s">
+        <v>1371</v>
+      </c>
+      <c r="O364" t="s">
+        <v>1370</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O360"/>
+  <autoFilter ref="A1:O364"/>
+  <hyperlinks>
+    <hyperlink ref="F363" r:id="rId1" display="http://algaebase.org/browse/taxonomy/?id=77642"/>
+    <hyperlink ref="E363" r:id="rId2" display="http://algaebase.org/browse/taxonomy/?id=139129"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -16555,22 +16678,22 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C1" t="s">
         <v>1353</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1354</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1355</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1356</v>
       </c>
-      <c r="F1" t="s">
-        <v>1357</v>
-      </c>
       <c r="G1" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -16677,7 +16800,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -16748,7 +16871,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -16769,7 +16892,7 @@
       </c>
       <c r="F19" s="35"/>
       <c r="G19" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -16782,7 +16905,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -16790,7 +16913,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -16826,19 +16949,19 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C1" t="s">
         <v>1353</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1354</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1355</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1356</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1357</v>
       </c>
       <c r="G1" s="32"/>
     </row>
@@ -16897,7 +17020,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
@@ -16962,7 +17085,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="33"/>
@@ -17008,7 +17131,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="33"/>
@@ -17051,37 +17174,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1281</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1282</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>1297</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>1299</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>1283</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>1288</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>1298</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="J1" t="s">
         <v>1300</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>1284</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>1289</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1299</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1301</v>
-      </c>
       <c r="K1" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -17089,7 +17212,7 @@
         <v>116</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
@@ -17106,7 +17229,7 @@
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -17114,7 +17237,7 @@
         <v>122</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -17127,7 +17250,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -17135,7 +17258,7 @@
         <v>127</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -17150,7 +17273,7 @@
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -17158,7 +17281,7 @@
         <v>132</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -17173,15 +17296,15 @@
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -17194,7 +17317,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
@@ -17202,7 +17325,7 @@
         <v>164</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9">
@@ -17217,7 +17340,7 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -17225,7 +17348,7 @@
         <v>88</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="11"/>
@@ -17238,7 +17361,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -17246,7 +17369,7 @@
         <v>140</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="11"/>
@@ -17259,15 +17382,15 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="11"/>
@@ -17280,15 +17403,15 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>1291</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>1292</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
@@ -17301,15 +17424,15 @@
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>1293</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>1294</v>
       </c>
       <c r="C12" s="9">
         <v>1</v>
@@ -17328,7 +17451,7 @@
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -17336,7 +17459,7 @@
         <v>1107</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9">
@@ -17349,7 +17472,7 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -17357,7 +17480,7 @@
         <v>178</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="12"/>
@@ -17370,15 +17493,15 @@
         <v>1</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>1297</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>1298</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
@@ -17391,12 +17514,12 @@
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="14" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
   </sheetData>
@@ -17472,7 +17595,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>168</v>
@@ -17488,7 +17611,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>116</v>
@@ -17496,47 +17619,47 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>1306</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>1307</v>
       </c>
       <c r="C8" s="27"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>116</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>127</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -17544,13 +17667,13 @@
         <v>1091</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="D12" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -17561,34 +17684,34 @@
         <v>116</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="D13" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>175</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>116</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
@@ -17599,10 +17722,10 @@
         <v>168</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.25" x14ac:dyDescent="0.35">
@@ -17613,211 +17736,211 @@
         <v>168</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D17" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>1306</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>1307</v>
       </c>
       <c r="C25" s="27"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>1316</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>1317</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>1318</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>1319</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>1320</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>1321</v>
       </c>
       <c r="C28" s="25"/>
       <c r="D28" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>1322</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>1323</v>
       </c>
       <c r="C29" s="25"/>
       <c r="D29" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>1324</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>1325</v>
       </c>
       <c r="C30" s="25"/>
       <c r="D30" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>1326</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>1327</v>
       </c>
       <c r="C31" s="25"/>
       <c r="D31" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B32" s="16" t="s">
         <v>1328</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>1329</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B33" s="22" t="s">
         <v>1330</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>1331</v>
       </c>
       <c r="C33" s="30"/>
       <c r="D33" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B34" s="16" t="s">
         <v>1332</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>1333</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B35" s="18" t="s">
         <v>1334</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>1335</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B36" s="16" t="s">
         <v>1336</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>1337</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B37" s="18" t="s">
         <v>1338</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>1339</v>
       </c>
       <c r="C37" s="25"/>
       <c r="D37" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B38" s="16" t="s">
         <v>1340</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>1341</v>
       </c>
       <c r="C38" s="25"/>
       <c r="D38" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>1342</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>1343</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B40" s="16" t="s">
         <v>1344</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>1345</v>
       </c>
       <c r="C40" s="25"/>
       <c r="D40" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="23" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B41" s="23" t="s">
         <v>1346</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>1347</v>
       </c>
       <c r="C41" s="31"/>
       <c r="D41" s="24" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
two corrections to toxin table
</commit_message>
<xml_diff>
--- a/output/nla_phyto_taxonomy.xlsx
+++ b/output/nla_phyto_taxonomy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13995" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13995" windowHeight="7500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="nla_phyto_taxonomy" sheetId="1" r:id="rId1"/>
@@ -293,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3582" uniqueCount="1376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3582" uniqueCount="1374">
   <si>
     <t>phylum</t>
   </si>
@@ -4670,12 +4670,6 @@
   </si>
   <si>
     <t>Pseudoanabaena</t>
-  </si>
-  <si>
-    <t>Synechococcusb</t>
-  </si>
-  <si>
-    <t>Synechocystisb</t>
   </si>
   <si>
     <t>Fischerella</t>
@@ -5777,9 +5771,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O364"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="G124" sqref="G124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11422,19 +11416,19 @@
         <v>1039</v>
       </c>
       <c r="G186" t="s">
+        <v>1370</v>
+      </c>
+      <c r="I186" t="s">
         <v>1372</v>
       </c>
-      <c r="I186" t="s">
-        <v>1374</v>
-      </c>
       <c r="J186" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K186" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="O186" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.25">
@@ -11454,19 +11448,19 @@
         <v>193</v>
       </c>
       <c r="G187" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="I187" t="s">
         <v>161</v>
       </c>
       <c r="J187" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="K187" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="O187" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.25">
@@ -11489,19 +11483,19 @@
         <v>313</v>
       </c>
       <c r="G188" t="s">
+        <v>1365</v>
+      </c>
+      <c r="I188" t="s">
         <v>1367</v>
       </c>
-      <c r="I188" t="s">
-        <v>1369</v>
-      </c>
       <c r="J188" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="K188" s="1" t="s">
         <v>34</v>
       </c>
       <c r="O188" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.25">
@@ -15336,7 +15330,7 @@
         <v>815</v>
       </c>
       <c r="G319" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="H319" t="s">
         <v>1018</v>
@@ -16681,11 +16675,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O364">
-    <sortState ref="A2:O364">
-      <sortCondition ref="G1:G364"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:O364"/>
   <hyperlinks>
     <hyperlink ref="F188" r:id="rId1" display="http://algaebase.org/browse/taxonomy/?id=77642"/>
     <hyperlink ref="E188" r:id="rId2" display="http://algaebase.org/browse/taxonomy/?id=139129"/>
@@ -16700,7 +16690,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16733,7 +16723,7 @@
         <v>1356</v>
       </c>
       <c r="G1" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -16840,7 +16830,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -16932,7 +16922,7 @@
       </c>
       <c r="F19" s="35"/>
       <c r="G19" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -16945,7 +16935,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1358</v>
+        <v>106</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -16953,7 +16943,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1359</v>
+        <v>79</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -17060,7 +17050,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
@@ -17171,7 +17161,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="33"/>
@@ -17194,8 +17184,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
another tox spelling corrected
</commit_message>
<xml_diff>
--- a/output/nla_phyto_taxonomy.xlsx
+++ b/output/nla_phyto_taxonomy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13995" windowHeight="7500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13995" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nla_phyto_taxonomy" sheetId="1" r:id="rId1"/>
@@ -293,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3582" uniqueCount="1374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3582" uniqueCount="1373">
   <si>
     <t>phylum</t>
   </si>
@@ -4667,9 +4667,6 @@
   </si>
   <si>
     <t>saxitoxin</t>
-  </si>
-  <si>
-    <t>Pseudoanabaena</t>
   </si>
   <si>
     <t>Fischerella</t>
@@ -11416,19 +11413,19 @@
         <v>1039</v>
       </c>
       <c r="G186" t="s">
+        <v>1369</v>
+      </c>
+      <c r="I186" t="s">
+        <v>1371</v>
+      </c>
+      <c r="J186" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K186" t="s">
+        <v>1372</v>
+      </c>
+      <c r="O186" t="s">
         <v>1370</v>
-      </c>
-      <c r="I186" t="s">
-        <v>1372</v>
-      </c>
-      <c r="J186" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K186" t="s">
-        <v>1373</v>
-      </c>
-      <c r="O186" t="s">
-        <v>1371</v>
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.25">
@@ -11448,19 +11445,19 @@
         <v>193</v>
       </c>
       <c r="G187" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="I187" t="s">
         <v>161</v>
       </c>
       <c r="J187" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="K187" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="O187" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.25">
@@ -11483,19 +11480,19 @@
         <v>313</v>
       </c>
       <c r="G188" t="s">
+        <v>1364</v>
+      </c>
+      <c r="I188" t="s">
+        <v>1366</v>
+      </c>
+      <c r="J188" t="s">
+        <v>1364</v>
+      </c>
+      <c r="K188" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O188" t="s">
         <v>1365</v>
-      </c>
-      <c r="I188" t="s">
-        <v>1367</v>
-      </c>
-      <c r="J188" t="s">
-        <v>1365</v>
-      </c>
-      <c r="K188" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O188" t="s">
-        <v>1366</v>
       </c>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.25">
@@ -15330,7 +15327,7 @@
         <v>815</v>
       </c>
       <c r="G319" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="H319" t="s">
         <v>1018</v>
@@ -16689,8 +16686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16723,7 +16720,7 @@
         <v>1356</v>
       </c>
       <c r="G1" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -16830,7 +16827,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -16901,7 +16898,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1357</v>
+        <v>206</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -16922,7 +16919,7 @@
       </c>
       <c r="F19" s="35"/>
       <c r="G19" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -17050,7 +17047,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
@@ -17161,7 +17158,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="33"/>
@@ -17184,7 +17181,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>

</xml_diff>